<commit_message>
added sentence/tokens of cluster into json
</commit_message>
<xml_diff>
--- a/resources/inputSample.xlsx
+++ b/resources/inputSample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="4420" yWindow="5880" windowWidth="25600" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>correctLabel</t>
   </si>
@@ -112,6 +112,10 @@
   </si>
   <si>
     <t>2008年6月9日、WWDC 2008の基調講演にて発表され、北米や欧州、オーストラリア、日本、香港など22地域で同年7月11日に発売された[4]。UMTS (W-CDMA)の規格で第3世代移動通信システム(3G)の通信に対応し、GPS搭載、MobileMe対応など、新たに機能が追加された。カラーはホワイトとブラックの2種類。容量は8GB（ブラックのみ）と16GBモデルが用意された。2010年6月24日に販売終了。</t>
+  </si>
+  <si>
+    <t>docIndex</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -488,220 +492,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>